<commit_message>
updated a bit of data in database exel
</commit_message>
<xml_diff>
--- a/Database .xlsx
+++ b/Database .xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="192">
   <si>
     <t>Commodity</t>
   </si>
@@ -364,9 +364,6 @@
     <t>Golden/White</t>
   </si>
   <si>
-    <t>retailer assigned (4591)</t>
-  </si>
-  <si>
     <t>Choy</t>
   </si>
   <si>
@@ -481,47 +478,122 @@
     <t>Brown</t>
   </si>
   <si>
-    <t>Black (4266)</t>
-  </si>
-  <si>
     <t>White/ Dried</t>
   </si>
   <si>
-    <t>Brown (4267)</t>
-  </si>
-  <si>
-    <t>White / Green (4268)</t>
-  </si>
-  <si>
-    <t>dried (3337)</t>
-  </si>
-  <si>
-    <t>retailer assigned (4269)</t>
+    <t>Retailed Assigned</t>
   </si>
   <si>
     <t>Garlic</t>
   </si>
   <si>
-    <t>Elephant (4609)</t>
-  </si>
-  <si>
-    <t>One-clove types (3401)</t>
-  </si>
-  <si>
-    <t>Regular (4608), fresh or semi-dried with leaves attached (3399), smoked (3400)</t>
-  </si>
-  <si>
-    <t>String (3052)</t>
-  </si>
-  <si>
-    <t>retailer assigned (4610-4611)</t>
+    <t>Elephant</t>
+  </si>
+  <si>
+    <t>On-clove Types</t>
+  </si>
+  <si>
+    <t>Sem-dried</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Ginger</t>
+  </si>
+  <si>
+    <t>Root</t>
+  </si>
+  <si>
+    <t>Gobo Root</t>
+  </si>
+  <si>
+    <t>Grape</t>
+  </si>
+  <si>
+    <t>Blue/Black Seeded</t>
+  </si>
+  <si>
+    <t>Champagne</t>
+  </si>
+  <si>
+    <t>Concord</t>
+  </si>
+  <si>
+    <t>Fantasy</t>
+  </si>
+  <si>
+    <t>Italian, Seeded</t>
+  </si>
+  <si>
+    <t>Red, Seeded</t>
+  </si>
+  <si>
+    <t>Autumn, Seedless</t>
+  </si>
+  <si>
+    <t>White/ Green Seeded</t>
+  </si>
+  <si>
+    <t>Grapefruit</t>
+  </si>
+  <si>
+    <t>Sweetie</t>
+  </si>
+  <si>
+    <t>Deep Red</t>
+  </si>
+  <si>
+    <t>Small-(Organic)</t>
+  </si>
+  <si>
+    <t>Large-(Organic)</t>
+  </si>
+  <si>
+    <t>Extra Large-(Organic)</t>
+  </si>
+  <si>
+    <t>Greens</t>
+  </si>
+  <si>
+    <t>Arugula / Rocket (4884)</t>
+  </si>
+  <si>
+    <t>Collards (4614)</t>
+  </si>
+  <si>
+    <t>Dandelion (4615)</t>
+  </si>
+  <si>
+    <t>Kale (4627), multicolor (3095)</t>
+  </si>
+  <si>
+    <t>Mustard (4616)</t>
+  </si>
+  <si>
+    <t>Polk Greens (4617)</t>
+  </si>
+  <si>
+    <t>Texas Mustard (4618)</t>
+  </si>
+  <si>
+    <t>Turnip (4619)</t>
+  </si>
+  <si>
+    <t>retailer assigned (4620-4624)</t>
+  </si>
+  <si>
+    <t>Guava</t>
+  </si>
+  <si>
+    <t>Guava (4299)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -536,18 +608,17 @@
       <name val="Arial"/>
     </font>
     <font>
-      <i/>
-      <color rgb="FF0A0000"/>
-      <name val="Inherit"/>
-    </font>
-    <font/>
-    <font>
       <b/>
       <sz val="11.0"/>
       <color rgb="FF0A0000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <color rgb="FF0A0000"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <i/>
       <color rgb="FF0A0000"/>
       <name val="Inherit"/>
     </font>
@@ -578,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -591,13 +662,10 @@
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -2650,16 +2718,13 @@
       <c r="D134" s="1">
         <v>4258.0</v>
       </c>
-      <c r="G134" s="3" t="s">
-        <v>117</v>
-      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B135" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="D135" s="1">
         <v>3163.0</v>
@@ -2667,13 +2732,13 @@
     </row>
     <row r="136">
       <c r="A136" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B136" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="D136" s="1">
         <v>4544.0</v>
@@ -2681,10 +2746,10 @@
     </row>
     <row r="137">
       <c r="A137" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B137" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>12</v>
@@ -2695,10 +2760,10 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>79</v>
@@ -2709,12 +2774,12 @@
     </row>
     <row r="139">
       <c r="A139" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C139" s="4" t="s">
+      <c r="C139" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D139" s="1">
@@ -2723,10 +2788,10 @@
     </row>
     <row r="140">
       <c r="A140" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>12</v>
@@ -2737,10 +2802,10 @@
     </row>
     <row r="141">
       <c r="A141" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>79</v>
@@ -2751,10 +2816,10 @@
     </row>
     <row r="142">
       <c r="A142" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>12</v>
@@ -2765,10 +2830,10 @@
     </row>
     <row r="143">
       <c r="A143" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>12</v>
@@ -2779,10 +2844,10 @@
     </row>
     <row r="144">
       <c r="A144" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B144" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>12</v>
@@ -2793,10 +2858,10 @@
     </row>
     <row r="145">
       <c r="A145" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>12</v>
@@ -2807,10 +2872,10 @@
     </row>
     <row r="146">
       <c r="A146" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>12</v>
@@ -2821,13 +2886,13 @@
     </row>
     <row r="147">
       <c r="A147" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B147" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="C147" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="D147" s="1">
         <v>3086.0</v>
@@ -2835,10 +2900,10 @@
     </row>
     <row r="148">
       <c r="A148" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>10</v>
@@ -2849,13 +2914,13 @@
     </row>
     <row r="149">
       <c r="A149" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="C149" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D149" s="1">
         <v>3087.0</v>
@@ -2863,13 +2928,13 @@
     </row>
     <row r="150">
       <c r="A150" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B150" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="C150" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D150" s="1">
         <v>4589.0</v>
@@ -2877,10 +2942,10 @@
     </row>
     <row r="151">
       <c r="A151" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B151" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>79</v>
@@ -2891,13 +2956,13 @@
     </row>
     <row r="152">
       <c r="A152" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B152" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="C152" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D152" s="1">
         <v>4590.0</v>
@@ -2905,10 +2970,10 @@
     </row>
     <row r="153">
       <c r="A153" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>24</v>
@@ -2919,10 +2984,10 @@
     </row>
     <row r="154">
       <c r="A154" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>45</v>
@@ -2933,10 +2998,10 @@
     </row>
     <row r="155">
       <c r="A155" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>12</v>
@@ -2947,10 +3012,10 @@
     </row>
     <row r="156">
       <c r="A156" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>12</v>
@@ -2961,13 +3026,13 @@
     </row>
     <row r="157">
       <c r="A157" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D157" s="1">
         <v>4062.0</v>
@@ -2975,10 +3040,10 @@
     </row>
     <row r="158">
       <c r="A158" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>24</v>
@@ -2989,10 +3054,10 @@
     </row>
     <row r="159">
       <c r="A159" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>12</v>
@@ -3003,10 +3068,10 @@
     </row>
     <row r="160">
       <c r="A160" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>12</v>
@@ -3017,7 +3082,7 @@
     </row>
     <row r="161">
       <c r="A161" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>12</v>
@@ -3031,13 +3096,13 @@
     </row>
     <row r="162">
       <c r="A162" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C162" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="D162" s="1">
         <v>3305.0</v>
@@ -3045,7 +3110,7 @@
     </row>
     <row r="163">
       <c r="A163" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>12</v>
@@ -3059,10 +3124,10 @@
     </row>
     <row r="164">
       <c r="A164" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B164" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>12</v>
@@ -3073,13 +3138,13 @@
     </row>
     <row r="165">
       <c r="A165" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D165" s="1">
         <v>3045.0</v>
@@ -3087,10 +3152,10 @@
     </row>
     <row r="166">
       <c r="A166" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>12</v>
@@ -3101,12 +3166,12 @@
     </row>
     <row r="167">
       <c r="A167" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C167" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C167" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D167" s="1">
@@ -3115,7 +3180,7 @@
     </row>
     <row r="168">
       <c r="A168" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>17</v>
@@ -3129,7 +3194,7 @@
     </row>
     <row r="169">
       <c r="A169" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>17</v>
@@ -3143,7 +3208,7 @@
     </row>
     <row r="170">
       <c r="A170" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>17</v>
@@ -3157,7 +3222,7 @@
     </row>
     <row r="171">
       <c r="A171" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>79</v>
@@ -3184,7 +3249,7 @@
     </row>
     <row r="174">
       <c r="B174" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D174" s="1">
         <v>4601.0</v>
@@ -3194,15 +3259,15 @@
       <c r="B175" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D175" s="4">
+      <c r="D175" s="1">
         <v>4081.0</v>
       </c>
     </row>
     <row r="176">
       <c r="B176" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D176" s="4">
+        <v>150</v>
+      </c>
+      <c r="D176" s="1">
         <v>3090.0</v>
       </c>
     </row>
@@ -3210,7 +3275,7 @@
       <c r="B177" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D177" s="4">
+      <c r="D177" s="1">
         <v>4602.0</v>
       </c>
     </row>
@@ -3224,15 +3289,15 @@
     </row>
     <row r="179">
       <c r="A179" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D179" s="1">
         <v>4265.0</v>
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="4" t="s">
-        <v>153</v>
+      <c r="A180" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="D180" s="1">
         <v>4606.0</v>
@@ -3240,80 +3305,468 @@
     </row>
     <row r="181">
       <c r="A181" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D181" s="1">
+        <v>4266.0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C182" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B181" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G181" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="C182" s="1" t="s">
+      <c r="D182" s="1">
+        <v>4267.0</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C183" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G182" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="C183" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="G183" s="6" t="s">
-        <v>158</v>
+      <c r="D183" s="1">
+        <v>4268.0</v>
       </c>
     </row>
     <row r="184">
+      <c r="A184" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C184" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G184" s="6" t="s">
+      <c r="D184" s="1">
+        <v>3337.0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D185" s="1">
+        <v>4269.0</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D186" s="1">
+        <v>4609.0</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="B187" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="185">
-      <c r="G185" s="3" t="s">
+      <c r="D187" s="1">
+        <v>3401.0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="B188" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D188" s="1">
+        <v>4608.0</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="B189" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="186">
-      <c r="G186" s="3" t="s">
+      <c r="D189" s="1">
+        <v>3399.0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="B190" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="187">
-      <c r="G187" s="5" t="s">
+      <c r="D190" s="1">
+        <v>3052.0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="188">
-      <c r="G188" s="6" t="s">
+      <c r="B191" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="189">
-      <c r="G189" s="6" t="s">
+      <c r="C191" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D191" s="1">
+        <v>4612.0</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="B192" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D192" s="1">
+        <v>4613.0</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="190">
-      <c r="G190" s="6" t="s">
+      <c r="D193" s="1">
+        <v>3091.0</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="191">
-      <c r="G191" s="6" t="s">
+      <c r="B194" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="192">
-      <c r="G192" s="3" t="s">
+      <c r="D194" s="1">
+        <v>4270.0</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="B195" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D195" s="1">
+        <v>4957.0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="B196" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D196" s="1">
+        <v>4056.0</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="B197" s="1" t="s">
         <v>167</v>
+      </c>
+      <c r="D197" s="1">
+        <v>4271.0</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="B198" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D198" s="1">
+        <v>4272.0</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="B199" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D199" s="1">
+        <v>4638.0</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="B200" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D200" s="1">
+        <v>3043.0</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="B201" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D201" s="1">
+        <v>4273.0</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="B202" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D202" s="1">
+        <v>4497.0</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="B203" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D203" s="1">
+        <v>4274.0</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="B204" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D204" s="1">
+        <v>4022.0</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="B205" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D205" s="1">
+        <v>4498.0</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D206" s="1">
+        <v>3092.0</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="B207" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D207" s="1">
+        <v>4285.0</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="C208" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D208" s="1">
+        <v>42841.0</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="C209" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D209" s="1">
+        <v>42862.0</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="C210" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D210" s="1">
+        <v>4288.0</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="C211" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D211" s="1">
+        <v>42892.0</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="C212" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D212" s="1">
+        <v>42871.0</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="C213" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D213" s="1">
+        <v>4492.0</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="C214" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D214" s="1">
+        <v>44911.0</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="C215" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D215" s="1">
+        <v>44932.0</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="B216" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D216" s="1">
+        <v>4291.0</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="C217" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D217" s="1">
+        <v>42901.0</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="C218" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D218" s="1">
+        <v>42922.0</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="C219" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D219" s="1">
+        <v>4294.0</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="C220" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D220" s="1">
+        <v>42931.0</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="C221" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D221" s="1">
+        <v>42952.0</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="C222" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D222" s="1">
+        <v>3159.0</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="C223" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D223" s="1">
+        <v>31571.0</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="C224" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D224" s="1">
+        <v>315582.0</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F225" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="F226" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="F227" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="F228" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="F229" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="F230" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="F231" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="F232" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="F233" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="F234" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="F235" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="F236" s="4" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>